<commit_message>
all mvc ready without update
</commit_message>
<xml_diff>
--- a/db_meta.xlsx
+++ b/db_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LazyCROW\Documents\Argusoft Workspace\Employee-Mng-Sys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE639627-8525-4C51-828E-F2D417C6F627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5765DF5-07C0-4212-B6A2-C0D1496B8928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>